<commit_message>
Added bo and page model
</commit_message>
<xml_diff>
--- a/src/test/resources/Login.xlsx
+++ b/src/test/resources/Login.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Data1</t>
   </si>
@@ -41,20 +41,23 @@
     <t>password</t>
   </si>
   <si>
-    <t>admin2</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
-    <t>admin ii</t>
+    <t>petroandrushchak@gmail.com</t>
+  </si>
+  <si>
+    <t>Petro</t>
+  </si>
+  <si>
+    <t>2change!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -201,6 +204,12 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="17">
@@ -432,7 +441,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -475,8 +484,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -485,8 +495,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% – Акцентування1" xfId="3" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% – Акцентування2" xfId="5" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% – Акцентування3" xfId="2" builtinId="38" customBuiltin="1"/>
@@ -512,6 +523,7 @@
     <cellStyle name="Акцентування5" xfId="28" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Акцентування6" xfId="29" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ввід" xfId="38" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Гіперпосилання" xfId="42" builtinId="8"/>
     <cellStyle name="Добре" xfId="19" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Заголовок 1" xfId="35" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Заголовок 2" xfId="32" builtinId="17" customBuiltin="1"/>
@@ -894,7 +906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,7 +917,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,17 +967,17 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,8 +1117,11 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>